<commit_message>
novo arquivo sem fundo
</commit_message>
<xml_diff>
--- a/Controle_de_producao.xlsx
+++ b/Controle_de_producao.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Novo Lar\Atividades\Excel\Aula12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0C4E65-A2FC-422C-9B3C-AB79D7AE9DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FFE105-D43B-4E8C-A06D-0A8A69E3945A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,30 +124,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -177,29 +159,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J17" sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +496,7 @@
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,303 +508,353 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>35</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>42</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>35</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>45</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>51</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>36</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>40</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>36</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>44</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>52</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>30</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>39</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>37</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>42</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>50</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>29</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>38</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>33</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>48</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>49</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>27</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>35</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>35</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>47</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>48</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>35</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>36</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>34</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>46</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>46</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="3">
         <v>32</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>43</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>32</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>42</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>52</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>30</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>25</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>38</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>41</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>53</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>29</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>45</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>38</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>45</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>50</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>28</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>42</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>35</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>46</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>49</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="3">
         <v>33</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>41</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>32</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>48</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>48</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>